<commit_message>
Login es el archivo principal con la nueva Interfaz Grafica
</commit_message>
<xml_diff>
--- a/Formatollenado.xlsx
+++ b/Formatollenado.xlsx
@@ -502,9 +502,9 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col width="8" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
-    <col width="8" customWidth="1" style="3" min="2" max="2"/>
-    <col width="2" customWidth="1" style="3" min="3" max="3"/>
-    <col width="2" customWidth="1" style="3" min="4" max="4"/>
+    <col width="17" customWidth="1" style="3" min="2" max="2"/>
+    <col width="11" customWidth="1" style="3" min="3" max="3"/>
+    <col width="10" customWidth="1" style="3" min="4" max="4"/>
     <col width="12" customWidth="1" style="3" min="5" max="9"/>
     <col width="12" customWidth="1" style="3" min="6" max="6"/>
     <col width="12" customWidth="1" style="3" min="7" max="7"/>
@@ -777,242 +777,1124 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="n"/>
-      <c r="B4" s="7" t="n"/>
-      <c r="C4" s="7" t="n"/>
-      <c r="D4" s="7" t="n"/>
-      <c r="E4" s="7" t="n"/>
-      <c r="F4" s="7" t="n"/>
-      <c r="G4" s="7" t="n"/>
-      <c r="H4" s="7" t="n"/>
-      <c r="I4" s="7" t="n"/>
-      <c r="J4" s="7" t="n"/>
-      <c r="K4" s="7" t="n"/>
-      <c r="L4" s="7" t="n"/>
-      <c r="M4" s="7" t="n"/>
-      <c r="N4" s="7" t="n"/>
-      <c r="O4" s="7" t="n"/>
-      <c r="P4" s="7" t="n"/>
-      <c r="Q4" s="7" t="n"/>
-      <c r="R4" s="7" t="n"/>
-      <c r="S4" s="7" t="n"/>
-      <c r="T4" s="7" t="n"/>
-      <c r="U4" s="7" t="n"/>
-      <c r="V4" s="7" t="n"/>
-      <c r="W4" s="7" t="n"/>
-      <c r="X4" s="7" t="n"/>
-      <c r="Y4" s="7" t="n"/>
-      <c r="Z4" s="7" t="n"/>
-      <c r="AA4" s="7" t="n"/>
-      <c r="AB4" s="7" t="n"/>
-      <c r="AC4" s="7" t="n"/>
-      <c r="AD4" s="7" t="n"/>
-      <c r="AE4" s="7" t="n"/>
-      <c r="AF4" s="7" t="n"/>
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>0005</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="inlineStr">
+        <is>
+          <t>JESUS</t>
+        </is>
+      </c>
+      <c r="C4" s="7" t="inlineStr">
+        <is>
+          <t>GASPAR</t>
+        </is>
+      </c>
+      <c r="D4" s="7" t="inlineStr">
+        <is>
+          <t>DIAZ</t>
+        </is>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G4" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J4" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K4" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="W4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AC4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF4" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="n"/>
-      <c r="B5" s="7" t="n"/>
-      <c r="C5" s="7" t="n"/>
-      <c r="D5" s="7" t="n"/>
-      <c r="E5" s="7" t="n"/>
-      <c r="F5" s="7" t="n"/>
-      <c r="G5" s="7" t="n"/>
-      <c r="H5" s="7" t="n"/>
-      <c r="I5" s="7" t="n"/>
-      <c r="J5" s="7" t="n"/>
-      <c r="K5" s="7" t="n"/>
-      <c r="L5" s="7" t="n"/>
-      <c r="M5" s="7" t="n"/>
-      <c r="N5" s="7" t="n"/>
-      <c r="O5" s="7" t="n"/>
-      <c r="P5" s="7" t="n"/>
-      <c r="Q5" s="7" t="n"/>
-      <c r="R5" s="7" t="n"/>
-      <c r="S5" s="7" t="n"/>
-      <c r="T5" s="7" t="n"/>
-      <c r="U5" s="7" t="n"/>
-      <c r="V5" s="7" t="n"/>
-      <c r="W5" s="7" t="n"/>
-      <c r="X5" s="7" t="n"/>
-      <c r="Y5" s="7" t="n"/>
-      <c r="Z5" s="7" t="n"/>
-      <c r="AA5" s="7" t="n"/>
-      <c r="AB5" s="7" t="n"/>
-      <c r="AC5" s="7" t="n"/>
-      <c r="AD5" s="7" t="n"/>
-      <c r="AE5" s="7" t="n"/>
-      <c r="AF5" s="7" t="n"/>
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>0021</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>FELIPE DE JESUS</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>GASPAR</t>
+        </is>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>ZATARAIN</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G5" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I5" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J5" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K5" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="W5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AC5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF5" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="n"/>
-      <c r="B6" s="7" t="n"/>
-      <c r="C6" s="7" t="n"/>
-      <c r="D6" s="7" t="n"/>
-      <c r="E6" s="7" t="n"/>
-      <c r="F6" s="7" t="n"/>
-      <c r="G6" s="7" t="n"/>
-      <c r="H6" s="7" t="n"/>
-      <c r="I6" s="7" t="n"/>
-      <c r="J6" s="7" t="n"/>
-      <c r="K6" s="7" t="n"/>
-      <c r="L6" s="7" t="n"/>
-      <c r="M6" s="7" t="n"/>
-      <c r="N6" s="7" t="n"/>
-      <c r="O6" s="7" t="n"/>
-      <c r="P6" s="7" t="n"/>
-      <c r="Q6" s="7" t="n"/>
-      <c r="R6" s="7" t="n"/>
-      <c r="S6" s="7" t="n"/>
-      <c r="T6" s="7" t="n"/>
-      <c r="U6" s="7" t="n"/>
-      <c r="V6" s="7" t="n"/>
-      <c r="W6" s="7" t="n"/>
-      <c r="X6" s="7" t="n"/>
-      <c r="Y6" s="7" t="n"/>
-      <c r="Z6" s="7" t="n"/>
-      <c r="AA6" s="7" t="n"/>
-      <c r="AB6" s="7" t="n"/>
-      <c r="AC6" s="7" t="n"/>
-      <c r="AD6" s="7" t="n"/>
-      <c r="AE6" s="7" t="n"/>
-      <c r="AF6" s="7" t="n"/>
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>0073</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="inlineStr">
+        <is>
+          <t>MARIO</t>
+        </is>
+      </c>
+      <c r="C6" s="7" t="inlineStr">
+        <is>
+          <t>ITURBIDE</t>
+        </is>
+      </c>
+      <c r="D6" s="7" t="inlineStr">
+        <is>
+          <t>VELARDE</t>
+        </is>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G6" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H6" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I6" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J6" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K6" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="W6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AC6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF6" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="n"/>
-      <c r="B7" s="7" t="n"/>
-      <c r="C7" s="7" t="n"/>
-      <c r="D7" s="7" t="n"/>
-      <c r="E7" s="7" t="n"/>
-      <c r="F7" s="7" t="n"/>
-      <c r="G7" s="7" t="n"/>
-      <c r="H7" s="7" t="n"/>
-      <c r="I7" s="7" t="n"/>
-      <c r="J7" s="7" t="n"/>
-      <c r="K7" s="7" t="n"/>
-      <c r="L7" s="7" t="n"/>
-      <c r="M7" s="7" t="n"/>
-      <c r="N7" s="7" t="n"/>
-      <c r="O7" s="7" t="n"/>
-      <c r="P7" s="7" t="n"/>
-      <c r="Q7" s="7" t="n"/>
-      <c r="R7" s="7" t="n"/>
-      <c r="S7" s="7" t="n"/>
-      <c r="T7" s="7" t="n"/>
-      <c r="U7" s="7" t="n"/>
-      <c r="V7" s="7" t="n"/>
-      <c r="W7" s="7" t="n"/>
-      <c r="X7" s="7" t="n"/>
-      <c r="Y7" s="7" t="n"/>
-      <c r="Z7" s="7" t="n"/>
-      <c r="AA7" s="7" t="n"/>
-      <c r="AB7" s="7" t="n"/>
-      <c r="AC7" s="7" t="n"/>
-      <c r="AD7" s="7" t="n"/>
-      <c r="AE7" s="7" t="n"/>
-      <c r="AF7" s="7" t="n"/>
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>0147</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="inlineStr">
+        <is>
+          <t>MISAEL</t>
+        </is>
+      </c>
+      <c r="C7" s="7" t="inlineStr">
+        <is>
+          <t>MARTINEZ</t>
+        </is>
+      </c>
+      <c r="D7" s="7" t="inlineStr">
+        <is>
+          <t>LIZAMA</t>
+        </is>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G7" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H7" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I7" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J7" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K7" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="W7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AC7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF7" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="n"/>
-      <c r="B8" s="7" t="n"/>
-      <c r="C8" s="7" t="n"/>
-      <c r="D8" s="7" t="n"/>
-      <c r="E8" s="7" t="n"/>
-      <c r="F8" s="7" t="n"/>
-      <c r="G8" s="7" t="n"/>
-      <c r="H8" s="7" t="n"/>
-      <c r="I8" s="7" t="n"/>
-      <c r="J8" s="7" t="n"/>
-      <c r="K8" s="7" t="n"/>
-      <c r="L8" s="7" t="n"/>
-      <c r="M8" s="7" t="n"/>
-      <c r="N8" s="7" t="n"/>
-      <c r="O8" s="7" t="n"/>
-      <c r="P8" s="7" t="n"/>
-      <c r="Q8" s="7" t="n"/>
-      <c r="R8" s="7" t="n"/>
-      <c r="S8" s="7" t="n"/>
-      <c r="T8" s="7" t="n"/>
-      <c r="U8" s="7" t="n"/>
-      <c r="V8" s="7" t="n"/>
-      <c r="W8" s="7" t="n"/>
-      <c r="X8" s="7" t="n"/>
-      <c r="Y8" s="7" t="n"/>
-      <c r="Z8" s="7" t="n"/>
-      <c r="AA8" s="7" t="n"/>
-      <c r="AB8" s="7" t="n"/>
-      <c r="AC8" s="7" t="n"/>
-      <c r="AD8" s="7" t="n"/>
-      <c r="AE8" s="7" t="n"/>
-      <c r="AF8" s="7" t="n"/>
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>0008</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="inlineStr">
+        <is>
+          <t>FRANCISCO</t>
+        </is>
+      </c>
+      <c r="C8" s="7" t="inlineStr">
+        <is>
+          <t>BARRETT</t>
+        </is>
+      </c>
+      <c r="D8" s="7" t="inlineStr">
+        <is>
+          <t>RAMOS</t>
+        </is>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G8" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H8" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I8" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J8" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K8" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="W8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AC8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF8" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="n"/>
-      <c r="B9" s="7" t="n"/>
-      <c r="C9" s="7" t="n"/>
-      <c r="D9" s="7" t="n"/>
-      <c r="E9" s="7" t="n"/>
-      <c r="F9" s="7" t="n"/>
-      <c r="G9" s="7" t="n"/>
-      <c r="H9" s="7" t="n"/>
-      <c r="I9" s="7" t="n"/>
-      <c r="J9" s="7" t="n"/>
-      <c r="K9" s="7" t="n"/>
-      <c r="L9" s="7" t="n"/>
-      <c r="M9" s="7" t="n"/>
-      <c r="N9" s="7" t="n"/>
-      <c r="O9" s="7" t="n"/>
-      <c r="P9" s="7" t="n"/>
-      <c r="Q9" s="7" t="n"/>
-      <c r="R9" s="7" t="n"/>
-      <c r="S9" s="7" t="n"/>
-      <c r="T9" s="7" t="n"/>
-      <c r="U9" s="7" t="n"/>
-      <c r="V9" s="7" t="n"/>
-      <c r="W9" s="7" t="n"/>
-      <c r="X9" s="7" t="n"/>
-      <c r="Y9" s="7" t="n"/>
-      <c r="Z9" s="7" t="n"/>
-      <c r="AA9" s="7" t="n"/>
-      <c r="AB9" s="7" t="n"/>
-      <c r="AC9" s="7" t="n"/>
-      <c r="AD9" s="7" t="n"/>
-      <c r="AE9" s="7" t="n"/>
-      <c r="AF9" s="7" t="n"/>
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>0064</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>CANDELARIO</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="inlineStr">
+        <is>
+          <t>GONZALEZ</t>
+        </is>
+      </c>
+      <c r="D9" s="7" t="inlineStr">
+        <is>
+          <t>MEDRANO</t>
+        </is>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H9" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I9" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J9" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K9" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="W9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AC9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF9" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="n"/>
-      <c r="B10" s="7" t="n"/>
-      <c r="C10" s="7" t="n"/>
-      <c r="D10" s="7" t="n"/>
-      <c r="E10" s="7" t="n"/>
-      <c r="F10" s="7" t="n"/>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
-      <c r="I10" s="7" t="n"/>
-      <c r="J10" s="7" t="n"/>
-      <c r="K10" s="7" t="n"/>
-      <c r="L10" s="7" t="n"/>
-      <c r="M10" s="7" t="n"/>
-      <c r="N10" s="7" t="n"/>
-      <c r="O10" s="7" t="n"/>
-      <c r="P10" s="7" t="n"/>
-      <c r="Q10" s="7" t="n"/>
-      <c r="R10" s="7" t="n"/>
-      <c r="S10" s="7" t="n"/>
-      <c r="T10" s="7" t="n"/>
-      <c r="U10" s="7" t="n"/>
-      <c r="V10" s="7" t="n"/>
-      <c r="W10" s="7" t="n"/>
-      <c r="X10" s="7" t="n"/>
-      <c r="Y10" s="7" t="n"/>
-      <c r="Z10" s="7" t="n"/>
-      <c r="AA10" s="7" t="n"/>
-      <c r="AB10" s="7" t="n"/>
-      <c r="AC10" s="7" t="n"/>
-      <c r="AD10" s="7" t="n"/>
-      <c r="AE10" s="7" t="n"/>
-      <c r="AF10" s="7" t="n"/>
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>0146</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>CARLOS ENRIQUE</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr">
+        <is>
+          <t>GUTIERREZ</t>
+        </is>
+      </c>
+      <c r="D10" s="7" t="inlineStr">
+        <is>
+          <t>ARMENTA</t>
+        </is>
+      </c>
+      <c r="E10" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I10" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J10" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K10" s="7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="W10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AC10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF10" s="7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="n"/>

</xml_diff>